<commit_message>
Foi adicionado a tag <table> para enviar a tabela no corpo do email
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\PycharmProjects\emails\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\PycharmProjects\emails\maladireta_outlook_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFDF742-6F3F-46F2-8DB3-CE5277FBDD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DFA71B-0927-4FE4-A682-62DFF7DAA71C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0AF807C4-2250-41FA-B679-2BAE2A0B7558}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{0AF807C4-2250-41FA-B679-2BAE2A0B7558}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -468,7 +468,7 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -546,8 +546,8 @@
   <sheetPr codeName="Planilha2"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -581,8 +581,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{BA654EB3-AD41-464D-B5EC-6A743648CF32}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{F75A189F-DDB1-4C6D-A06A-417335DD1EF2}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D4F7D6F4-75C0-414A-ABB1-723B352BF8DA}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{FB151BAF-BAF8-42FB-9B2E-B82592890B46}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>